<commit_message>
Updated UMAP plots to there correct ones
</commit_message>
<xml_diff>
--- a/Statistical Normalisation/Actual Data Models/Models/Text Results/Contrastive-0.25.xlsx
+++ b/Statistical Normalisation/Actual Data Models/Models/Text Results/Contrastive-0.25.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nia Touko\Documents\GitHub\Towards-adaptable-prosthetics-through-Spiking-Networks\Statistical Normalisation\Actual Data Models\Models\Text Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97E9D7A4-2C19-4025-9C32-90FE97583EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381B7C5D-6711-4FB6-82EA-84EBE2500D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4725" yWindow="1215" windowWidth="21600" windowHeight="11295" xr2:uid="{29F306E2-6453-42EF-8CA9-E210388BE32E}"/>
   </bookViews>
   <sheets>
     <sheet name="StandardModels" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -995,15 +1008,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0990B76D-DC16-46F1-960E-9536933370CF}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1020,9 +1033,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -1037,9 +1050,9 @@
         <v>66.904861986829204</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1054,9 +1067,9 @@
         <v>65.866753816704801</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -1071,9 +1084,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -1088,9 +1101,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
@@ -1105,9 +1118,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -1122,9 +1135,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
@@ -1139,9 +1152,9 @@
         <v>53.085269873794999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
@@ -1156,9 +1169,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>32</v>
@@ -1173,9 +1186,9 @@
         <v>37.449251014979701</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>34</v>
@@ -1188,6 +1201,18 @@
       </c>
       <c r="E11" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f>E2+E3+E3+E5+E4+E9</f>
+        <v>371.39093846129066</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f>I12/6</f>
+        <v>61.898489743548446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>